<commit_message>
fixing register map, so I don't write int32 into 2 bytes
</commit_message>
<xml_diff>
--- a/firmware/registers.xlsx
+++ b/firmware/registers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shuri\Dropbox\Robotics\github\motor-driver\firmware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3C14224-D29C-427B-9D4F-FA9CB956000B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1523CAA5-2345-4C89-AE65-B1E58600C975}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8712" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -144,9 +144,6 @@
     <t>12-13</t>
   </si>
   <si>
-    <t>34-35</t>
-  </si>
-  <si>
     <t>Kp*10^7</t>
   </si>
   <si>
@@ -183,15 +180,6 @@
     <t>REG_STATUS</t>
   </si>
   <si>
-    <t>28-29</t>
-  </si>
-  <si>
-    <t>30-31</t>
-  </si>
-  <si>
-    <t>32-33</t>
-  </si>
-  <si>
     <t>REG_ENCODER1</t>
   </si>
   <si>
@@ -250,6 +238,18 @@
   </si>
   <si>
     <t>Max motor speed in encoder ticks/s. Required for PID</t>
+  </si>
+  <si>
+    <t>28-31</t>
+  </si>
+  <si>
+    <t>32-35</t>
+  </si>
+  <si>
+    <t>36-37</t>
+  </si>
+  <si>
+    <t>38-39</t>
   </si>
 </sst>
 </file>
@@ -520,6 +520,42 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -529,6 +565,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -537,45 +576,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -896,8 +896,8 @@
   </sheetPr>
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -914,7 +914,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="33" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B1" s="34"/>
       <c r="C1" s="34"/>
@@ -951,47 +951,47 @@
       <c r="F3" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="39" t="s">
+      <c r="G3" s="27" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C4" s="20" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E4" s="18" t="s">
         <v>17</v>
       </c>
       <c r="F4" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="G4" s="40" t="s">
-        <v>65</v>
+        <v>42</v>
+      </c>
+      <c r="G4" s="28" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="14" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C5" s="20" t="s">
         <v>1</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>17</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G5" s="40"/>
+        <v>44</v>
+      </c>
+      <c r="G5" s="28"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B6" s="17" t="s">
@@ -1007,9 +1007,9 @@
         <v>13</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="G6" s="41"/>
+        <v>70</v>
+      </c>
+      <c r="G6" s="29"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B7" s="17" t="s">
@@ -1025,9 +1025,9 @@
         <v>13</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G7" s="41"/>
+        <v>39</v>
+      </c>
+      <c r="G7" s="29"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B8" s="17" t="s">
@@ -1045,7 +1045,7 @@
       <c r="F8" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G8" s="41"/>
+      <c r="G8" s="29"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B9" s="17" t="s">
@@ -1063,11 +1063,11 @@
       <c r="F9" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G9" s="41"/>
+      <c r="G9" s="29"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B10" s="17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C10" s="20" t="s">
         <v>1</v>
@@ -1081,7 +1081,7 @@
       <c r="F10" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="G10" s="41"/>
+      <c r="G10" s="29"/>
     </row>
     <row r="11" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B11" s="17" t="s">
@@ -1091,16 +1091,16 @@
         <v>1</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G11" s="42" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -1111,36 +1111,36 @@
         <v>1</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G12" s="42"/>
     </row>
     <row r="13" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B13" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C13" s="20"/>
       <c r="D13" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>17</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="G13" s="43"/>
+        <v>68</v>
+      </c>
+      <c r="G13" s="30"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="24"/>
       <c r="B14" s="25" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C14" s="24" t="s">
         <v>1</v>
@@ -1154,12 +1154,12 @@
       <c r="F14" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="G14" s="44" t="s">
-        <v>67</v>
+      <c r="G14" s="31" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="30" t="s">
+      <c r="A15" s="43" t="s">
         <v>15</v>
       </c>
       <c r="B15" s="4" t="s">
@@ -1177,10 +1177,10 @@
       <c r="F15" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G15" s="40"/>
+      <c r="G15" s="28"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="31"/>
+      <c r="A16" s="44"/>
       <c r="B16" s="7" t="s">
         <v>24</v>
       </c>
@@ -1194,10 +1194,10 @@
       <c r="F16" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="G16" s="40"/>
+      <c r="G16" s="28"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="31"/>
+      <c r="A17" s="44"/>
       <c r="B17" s="7" t="s">
         <v>25</v>
       </c>
@@ -1211,12 +1211,12 @@
         <v>7</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="G17" s="40"/>
+        <v>49</v>
+      </c>
+      <c r="G17" s="28"/>
     </row>
     <row r="18" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="32"/>
+      <c r="A18" s="45"/>
       <c r="B18" s="10" t="s">
         <v>26</v>
       </c>
@@ -1224,93 +1224,93 @@
         <v>5</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E18" s="11" t="s">
         <v>7</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="G18" s="45"/>
+        <v>65</v>
+      </c>
+      <c r="G18" s="32"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="27" t="s">
+      <c r="A19" s="39" t="s">
         <v>16</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>52</v>
+        <v>71</v>
       </c>
       <c r="C19" s="21" t="s">
         <v>5</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>11</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="G19" s="40"/>
+        <v>57</v>
+      </c>
+      <c r="G19" s="28"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="28"/>
+      <c r="A20" s="40"/>
       <c r="B20" s="7" t="s">
-        <v>53</v>
+        <v>72</v>
       </c>
       <c r="C20" s="22" t="s">
         <v>5</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E20" s="8" t="s">
         <v>11</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="G20" s="40"/>
+        <v>58</v>
+      </c>
+      <c r="G20" s="28"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="28"/>
+      <c r="A21" s="40"/>
       <c r="B21" s="7" t="s">
-        <v>54</v>
+        <v>73</v>
       </c>
       <c r="C21" s="22" t="s">
         <v>5</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E21" s="8" t="s">
         <v>12</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="G21" s="40"/>
+        <v>59</v>
+      </c>
+      <c r="G21" s="28"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="29"/>
+      <c r="A22" s="41"/>
       <c r="B22" s="10" t="s">
-        <v>39</v>
+        <v>74</v>
       </c>
       <c r="C22" s="23" t="s">
         <v>5</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E22" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="G22" s="45"/>
+        <v>60</v>
+      </c>
+      <c r="G22" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
Renaming to PRMC. Fixing enable in firmware
</commit_message>
<xml_diff>
--- a/firmware/registers.xlsx
+++ b/firmware/registers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shuri\Dropbox\Robotics\github\motor-driver\firmware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{456A3752-6A21-4A69-9CF3-5ED848C23035}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F9DF3A8-7DCD-40D4-9FA0-C969B4230FF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2370" yWindow="430" windowWidth="15120" windowHeight="9550" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="380" yWindow="380" windowWidth="16740" windowHeight="9550" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -147,9 +147,6 @@
     <t>REG_ENABLE</t>
   </si>
   <si>
-    <t>write 1 to enable motor drivers, 0 to disable</t>
-  </si>
-  <si>
     <t>0</t>
   </si>
   <si>
@@ -238,6 +235,9 @@
   </si>
   <si>
     <t xml:space="preserve">Register list. All multibyte registers use little-endian encoding; e.g. for register REG_POWER1, low byte is at address 12, and high byte, at address 13. </t>
+  </si>
+  <si>
+    <t>Bit0 is motor1, bit1 is motor2. set bit to 1 to enable motor driver, to 0 to disable</t>
   </si>
 </sst>
 </file>
@@ -867,7 +867,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -884,7 +884,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B1" s="30"/>
       <c r="C1" s="30"/>
@@ -925,9 +925,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" s="14" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="B4" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C4" s="20" t="s">
         <v>1</v>
@@ -939,10 +939,10 @@
         <v>17</v>
       </c>
       <c r="F4" s="19" t="s">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="G4" s="25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="14" customFormat="1" ht="29" x14ac:dyDescent="0.35">
@@ -953,13 +953,13 @@
         <v>1</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>17</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G5" s="25"/>
     </row>
@@ -977,7 +977,7 @@
         <v>13</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G6" s="26"/>
     </row>
@@ -1037,7 +1037,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B10" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C10" s="20" t="s">
         <v>1</v>
@@ -1061,16 +1061,16 @@
         <v>1</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G11" s="38" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
@@ -1081,29 +1081,29 @@
         <v>1</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G12" s="38"/>
     </row>
     <row r="13" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="B13" s="17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C13" s="20"/>
       <c r="D13" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>17</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G13" s="27"/>
     </row>
@@ -1160,7 +1160,7 @@
         <v>7</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G16" s="25"/>
     </row>
@@ -1173,13 +1173,13 @@
         <v>5</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E17" s="11" t="s">
         <v>7</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G17" s="28"/>
     </row>
@@ -1188,76 +1188,76 @@
         <v>16</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C18" s="21" t="s">
         <v>5</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>11</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G18" s="25"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="36"/>
       <c r="B19" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C19" s="22" t="s">
         <v>5</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E19" s="8" t="s">
         <v>11</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G19" s="25"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="36"/>
       <c r="B20" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C20" s="22" t="s">
         <v>5</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E20" s="8" t="s">
         <v>12</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G20" s="25"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="37"/>
       <c r="B21" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C21" s="23" t="s">
         <v>5</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E21" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G21" s="28"/>
     </row>

</xml_diff>